<commit_message>
a whole lot more steering committee documentation and reports
git-svn-id: svn://localhost/ARK/trunk@8255 35ee9b83-dd2c-47f4-99a2-c706670c48ce
</commit_message>
<xml_diff>
--- a/usefulTools/TestFilesAndDocuments/steering committee/NeCTAR/NeCTAR Reporting/NeCTAR Report RT029 30June2013 .xlsx
+++ b/usefulTools/TestFilesAndDocuments/steering committee/NeCTAR/NeCTAR Reporting/NeCTAR Report RT029 30June2013 .xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="23515"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="32720" windowHeight="20560" firstSheet="1" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="32700" windowHeight="20560" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="1.Header" sheetId="1" r:id="rId1"/>
@@ -269,7 +269,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="399">
   <si>
     <t>1.Header</t>
   </si>
@@ -543,9 +543,6 @@
     <t>Pedigree Storage &amp; Visualisation Module</t>
   </si>
   <si>
-    <t>Have completed design work and database schema changes. Have also identified suitable pedigree visualisation tool for integration.</t>
-  </si>
-  <si>
     <t>Funding Milestone 4</t>
   </si>
   <si>
@@ -568,9 +565,6 @@
   </si>
   <si>
     <t>Integrate Genotypic Data Management Capability</t>
-  </si>
-  <si>
-    <t>please note that none of these dates take into account the change request we submitted, but we are back on target for those amended dates</t>
   </si>
   <si>
     <t>Funding Milestone 5</t>
@@ -1499,9 +1493,6 @@
     <t>completed, signed off</t>
   </si>
   <si>
-    <t>Approx 90% complete as Data Extraction is the majority of this milestone.</t>
-  </si>
-  <si>
     <t>http://thearktools.blogspot.com.au/</t>
   </si>
   <si>
@@ -1523,9 +1514,6 @@
     <t>daily</t>
   </si>
   <si>
-    <t>Implemented and tested sub-study management capability to allow subjects from a parent study to be allocated to sub-studies without duplicating core subject data.  Subproject concept is documented and within the UAT documents for Nik Zeps and ATR.  Travis believes this may need separate UAT document, but this functionality has been coded, tested and signed off as part of initial production release by WARTN Team.    Note the dates are wrong due to cell validation rules...actual date was 28/03/2013.  Added additional signoff documents 7/8/13 in order to make sure we met all NECTaR requirements</t>
-  </si>
-  <si>
     <t>One developer has been ill and may need extended sick leave.  Have submitted an RFC to adjust milestone dates and have identified another part time develop to assist.  Developer did take leave, cannot be sure of the future availability of developer, but as of today he is back.  A tight timeline still exists, and part-time developer has not had the time available initially indicated to us. In the interim an increased output from some key members has allowed the project to make up for this shortfall as staff roll back into productivity.  A member of UWA team took on an extra day a week and has worked significantly over time to get back on (revised) schedule.  PhD student Thilina is also having to adjust his schedule to meet his writing and other needs, so his availability is a little less than originally thought but his productivity is still good at times he is available</t>
   </si>
   <si>
@@ -1542,6 +1530,24 @@
   </si>
   <si>
     <t>1.1.1d</t>
+  </si>
+  <si>
+    <t>Project manager is now Travis Endersby (travis.endersby@uwa.edu.au).  Significant steps have been made in catching up to revised deadlines you received 18 Feb.   Still on target for agreed upon target, although the completion of one module had to be delayed and one module was brought forward in its place.</t>
+  </si>
+  <si>
+    <t>Have completed design work and database schema changes. Have also identified &amp; are utilizing suitable pedigree visualisation tool for integration.  Just finalizing integration/presentation of the data beyond picture-based visualization of uploads to be manipulatable and presented in text/table formats</t>
+  </si>
+  <si>
+    <t>In reality approx 90-95% complete as Data Extraction is the majority of this milestone.</t>
+  </si>
+  <si>
+    <t>Implemented and tested sub-study management capability to allow subjects from a parent study to be allocated to sub-studies without duplicating core subject data.  This functionality had been coded, tested and signed off as part of initial production release by WARTN Team.     Added additional individual signoff documents 7/8/13 in order to make sure we met all NECTaR requirements</t>
+  </si>
+  <si>
+    <t>Started, designed.  Probably more like 15% right now, but wanted to indicate started and that is the best this worksheet offers</t>
+  </si>
+  <si>
+    <t>Travis Endersby</t>
   </si>
 </sst>
 </file>
@@ -2862,13 +2868,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="518">
+  <cellXfs count="519">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -4144,11 +4152,16 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="78" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="6">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1971">
@@ -32034,7 +32047,7 @@
   <dimension ref="A1:AI45"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35:N35"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -32641,7 +32654,9 @@
       </c>
     </row>
     <row r="35" spans="2:23" ht="88" customHeight="1">
-      <c r="B35" s="462"/>
+      <c r="B35" s="462" t="s">
+        <v>393</v>
+      </c>
       <c r="C35" s="463"/>
       <c r="D35" s="463"/>
       <c r="E35" s="463"/>
@@ -32758,7 +32773,9 @@
       <c r="C41" s="62"/>
       <c r="D41" s="62"/>
       <c r="E41" s="64"/>
-      <c r="F41" s="465"/>
+      <c r="F41" s="465" t="s">
+        <v>398</v>
+      </c>
       <c r="G41" s="466"/>
       <c r="H41" s="466"/>
       <c r="I41" s="466"/>
@@ -32779,7 +32796,9 @@
       <c r="C42" s="64"/>
       <c r="D42" s="64"/>
       <c r="E42" s="64"/>
-      <c r="F42" s="468"/>
+      <c r="F42" s="468">
+        <v>41469</v>
+      </c>
       <c r="G42" s="469"/>
       <c r="H42" s="469"/>
       <c r="I42" s="469"/>
@@ -32792,7 +32811,7 @@
     <row r="43" spans="2:23" ht="30" customHeight="1">
       <c r="B43" s="178" t="str">
         <f>IF(ISBLANK(F41),"Please signoff (select Yes and enter name) prior to form submission",IF(COUNTIF(T38:T40,"FALSE")&gt;0,"Please select Yes in signoff prior to form submission",""))</f>
-        <v>Please signoff (select Yes and enter name) prior to form submission</v>
+        <v/>
       </c>
       <c r="C43" s="65"/>
       <c r="D43" s="65"/>
@@ -35637,9 +35656,7 @@
   </sheetPr>
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
@@ -35742,13 +35759,13 @@
     <row r="12" spans="1:6" ht="28" customHeight="1">
       <c r="C12" s="5"/>
       <c r="D12" s="155" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E12" s="156" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F12" s="157" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="27" customHeight="1">
@@ -35756,7 +35773,7 @@
         <v>10</v>
       </c>
       <c r="D13" s="490" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E13" s="490"/>
       <c r="F13" s="490"/>
@@ -35766,13 +35783,13 @@
         <v>1</v>
       </c>
       <c r="D14" s="151" t="s">
+        <v>247</v>
+      </c>
+      <c r="E14" s="152" t="s">
+        <v>248</v>
+      </c>
+      <c r="F14" s="153" t="s">
         <v>249</v>
-      </c>
-      <c r="E14" s="152" t="s">
-        <v>250</v>
-      </c>
-      <c r="F14" s="153" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="28" customHeight="1">
@@ -35780,13 +35797,13 @@
         <v>2</v>
       </c>
       <c r="D15" s="151" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="E15" s="152" t="s">
+        <v>248</v>
+      </c>
+      <c r="F15" s="153" t="s">
         <v>250</v>
-      </c>
-      <c r="F15" s="153" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="28" customHeight="1">
@@ -35794,13 +35811,13 @@
         <v>3</v>
       </c>
       <c r="D16" s="151" t="s">
+        <v>251</v>
+      </c>
+      <c r="E16" s="152" t="s">
+        <v>252</v>
+      </c>
+      <c r="F16" s="153" t="s">
         <v>253</v>
-      </c>
-      <c r="E16" s="152" t="s">
-        <v>254</v>
-      </c>
-      <c r="F16" s="153" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="17" spans="3:6" ht="28" customHeight="1">
@@ -35808,13 +35825,13 @@
         <v>4</v>
       </c>
       <c r="D17" s="151" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="E17" s="152" t="s">
+        <v>248</v>
+      </c>
+      <c r="F17" s="153" t="s">
         <v>250</v>
-      </c>
-      <c r="F17" s="153" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="18" spans="3:6" ht="28" customHeight="1">
@@ -35822,13 +35839,13 @@
         <v>5</v>
       </c>
       <c r="D18" s="151" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E18" s="152" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F18" s="153" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="19" spans="3:6" ht="28" customHeight="1">
@@ -35836,13 +35853,13 @@
         <v>6</v>
       </c>
       <c r="D19" s="151" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E19" s="152" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F19" s="153" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="20" spans="3:6" ht="33" customHeight="1">
@@ -35850,13 +35867,13 @@
         <v>7</v>
       </c>
       <c r="D20" s="151" t="s">
+        <v>255</v>
+      </c>
+      <c r="E20" s="152" t="s">
+        <v>256</v>
+      </c>
+      <c r="F20" s="153" t="s">
         <v>257</v>
-      </c>
-      <c r="E20" s="152" t="s">
-        <v>258</v>
-      </c>
-      <c r="F20" s="153" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="21" spans="3:6" ht="60" customHeight="1">
@@ -35864,27 +35881,27 @@
         <v>8</v>
       </c>
       <c r="D21" s="151" t="s">
+        <v>258</v>
+      </c>
+      <c r="E21" s="152" t="s">
+        <v>259</v>
+      </c>
+      <c r="F21" s="153" t="s">
         <v>260</v>
-      </c>
-      <c r="E21" s="152" t="s">
-        <v>261</v>
-      </c>
-      <c r="F21" s="153" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="22" spans="3:6" ht="60" customHeight="1">
       <c r="C22" s="376" t="s">
+        <v>261</v>
+      </c>
+      <c r="D22" s="151" t="s">
+        <v>262</v>
+      </c>
+      <c r="E22" s="152" t="s">
         <v>263</v>
       </c>
-      <c r="D22" s="151" t="s">
+      <c r="F22" s="153" t="s">
         <v>264</v>
-      </c>
-      <c r="E22" s="152" t="s">
-        <v>265</v>
-      </c>
-      <c r="F22" s="153" t="s">
-        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -36087,48 +36104,48 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15" customHeight="1">
       <c r="A1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B1" t="s">
+        <v>265</v>
+      </c>
+      <c r="C1" t="s">
+        <v>266</v>
+      </c>
+      <c r="D1" t="s">
         <v>267</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>268</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>269</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>270</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" s="345" t="s">
         <v>271</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" s="345" t="s">
         <v>272</v>
-      </c>
-      <c r="H1" s="345" t="s">
-        <v>273</v>
-      </c>
-      <c r="I1" s="345" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1">
       <c r="A2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="F2" s="125">
         <v>40909</v>
@@ -36137,33 +36154,33 @@
         <v>42004</v>
       </c>
       <c r="H2" s="345" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="I2" s="345" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15" customHeight="1">
       <c r="A3" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B3">
         <v>25</v>
       </c>
       <c r="C3" t="s">
+        <v>277</v>
+      </c>
+      <c r="D3" t="s">
+        <v>127</v>
+      </c>
+      <c r="E3" t="s">
+        <v>214</v>
+      </c>
+      <c r="H3" s="345" t="s">
+        <v>278</v>
+      </c>
+      <c r="I3" s="345" t="s">
         <v>279</v>
-      </c>
-      <c r="D3" t="s">
-        <v>129</v>
-      </c>
-      <c r="E3" t="s">
-        <v>216</v>
-      </c>
-      <c r="H3" s="345" t="s">
-        <v>280</v>
-      </c>
-      <c r="I3" s="345" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15" customHeight="1">
@@ -36171,16 +36188,16 @@
         <v>50</v>
       </c>
       <c r="C4" t="s">
+        <v>280</v>
+      </c>
+      <c r="D4" t="s">
+        <v>245</v>
+      </c>
+      <c r="H4" s="345" t="s">
+        <v>281</v>
+      </c>
+      <c r="I4" s="345" t="s">
         <v>282</v>
-      </c>
-      <c r="D4" t="s">
-        <v>247</v>
-      </c>
-      <c r="H4" s="345" t="s">
-        <v>283</v>
-      </c>
-      <c r="I4" s="345" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1">
@@ -36188,11 +36205,11 @@
         <v>75</v>
       </c>
       <c r="C5" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H5" s="345"/>
       <c r="I5" s="345" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -36200,22 +36217,22 @@
         <v>100</v>
       </c>
       <c r="C6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="C7" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="8" spans="1:9" s="5" customFormat="1">
       <c r="C8" s="351" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="C9" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
   </sheetData>
@@ -36258,76 +36275,76 @@
         <v>16</v>
       </c>
       <c r="B1" s="233" t="s">
+        <v>287</v>
+      </c>
+      <c r="C1" s="234" t="s">
+        <v>288</v>
+      </c>
+      <c r="D1" s="234" t="s">
         <v>289</v>
       </c>
-      <c r="C1" s="234" t="s">
+      <c r="E1" s="234" t="s">
         <v>290</v>
       </c>
-      <c r="D1" s="234" t="s">
+      <c r="F1" s="234" t="s">
         <v>291</v>
       </c>
-      <c r="E1" s="234" t="s">
+      <c r="G1" s="235" t="s">
         <v>292</v>
       </c>
-      <c r="F1" s="234" t="s">
+      <c r="H1" s="236" t="s">
         <v>293</v>
       </c>
-      <c r="G1" s="235" t="s">
+      <c r="I1" s="237" t="s">
         <v>294</v>
       </c>
-      <c r="H1" s="236" t="s">
+      <c r="J1" s="235" t="s">
         <v>295</v>
       </c>
-      <c r="I1" s="237" t="s">
+      <c r="K1" s="236" t="s">
         <v>296</v>
       </c>
-      <c r="J1" s="235" t="s">
+      <c r="L1" s="237" t="s">
         <v>297</v>
       </c>
-      <c r="K1" s="236" t="s">
+      <c r="M1" s="235" t="s">
         <v>298</v>
       </c>
-      <c r="L1" s="237" t="s">
+      <c r="N1" s="236" t="s">
         <v>299</v>
       </c>
-      <c r="M1" s="235" t="s">
+      <c r="O1" s="237" t="s">
         <v>300</v>
       </c>
-      <c r="N1" s="236" t="s">
+      <c r="P1" s="238" t="s">
         <v>301</v>
       </c>
-      <c r="O1" s="237" t="s">
+      <c r="Q1" s="238" t="s">
         <v>302</v>
       </c>
-      <c r="P1" s="238" t="s">
+      <c r="R1" s="239" t="s">
         <v>303</v>
       </c>
-      <c r="Q1" s="238" t="s">
+      <c r="S1" s="239" t="s">
         <v>304</v>
       </c>
-      <c r="R1" s="239" t="s">
+      <c r="T1" s="239" t="s">
         <v>305</v>
       </c>
-      <c r="S1" s="239" t="s">
+      <c r="U1" s="247" t="s">
         <v>306</v>
       </c>
-      <c r="T1" s="239" t="s">
+      <c r="V1" s="248" t="s">
         <v>307</v>
       </c>
-      <c r="U1" s="247" t="s">
+      <c r="W1" s="248" t="s">
         <v>308</v>
       </c>
-      <c r="V1" s="248" t="s">
+      <c r="X1" s="248" t="s">
         <v>309</v>
       </c>
-      <c r="W1" s="248" t="s">
+      <c r="Y1" s="249" t="s">
         <v>310</v>
-      </c>
-      <c r="X1" s="248" t="s">
-        <v>311</v>
-      </c>
-      <c r="Y1" s="249" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="2" spans="1:25" ht="15" customHeight="1">
@@ -36908,7 +36925,7 @@
     </row>
     <row r="16" spans="1:25">
       <c r="U16" s="351" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
   </sheetData>
@@ -37113,7 +37130,7 @@
     <row r="15" spans="1:5" ht="19" customHeight="1">
       <c r="A15" s="65"/>
       <c r="B15" s="94" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C15" s="94"/>
       <c r="D15" s="94"/>
@@ -37122,7 +37139,7 @@
     <row r="16" spans="1:5" ht="16" customHeight="1">
       <c r="A16" s="65"/>
       <c r="B16" s="477" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C16" s="477"/>
       <c r="D16" s="477"/>
@@ -37130,7 +37147,7 @@
     </row>
     <row r="17" spans="2:10" ht="15" customHeight="1">
       <c r="B17" s="346" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="18" spans="2:10" s="5" customFormat="1" ht="15" customHeight="1">
@@ -37138,177 +37155,177 @@
     </row>
     <row r="19" spans="2:10" ht="32" customHeight="1">
       <c r="B19" s="347" t="s">
+        <v>315</v>
+      </c>
+      <c r="C19" s="347" t="s">
+        <v>316</v>
+      </c>
+      <c r="D19" s="347" t="s">
         <v>317</v>
       </c>
-      <c r="C19" s="347" t="s">
+      <c r="E19" s="347" t="s">
         <v>318</v>
       </c>
-      <c r="D19" s="347" t="s">
+      <c r="F19" s="347" t="s">
         <v>319</v>
       </c>
-      <c r="E19" s="347" t="s">
+      <c r="G19" s="347" t="s">
         <v>320</v>
       </c>
-      <c r="F19" s="347" t="s">
+      <c r="H19" s="347" t="s">
         <v>321</v>
       </c>
-      <c r="G19" s="347" t="s">
+      <c r="I19" s="347" t="s">
         <v>322</v>
       </c>
-      <c r="H19" s="347" t="s">
-        <v>323</v>
-      </c>
-      <c r="I19" s="347" t="s">
-        <v>324</v>
-      </c>
       <c r="J19" s="347" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="20" spans="2:10" ht="32" customHeight="1">
       <c r="B20" s="348" t="s">
+        <v>323</v>
+      </c>
+      <c r="C20" s="348" t="s">
+        <v>279</v>
+      </c>
+      <c r="D20" s="348" t="s">
+        <v>324</v>
+      </c>
+      <c r="E20" s="349" t="s">
         <v>325</v>
       </c>
-      <c r="C20" s="348" t="s">
-        <v>281</v>
-      </c>
-      <c r="D20" s="348" t="s">
+      <c r="F20" s="348" t="s">
         <v>326</v>
-      </c>
-      <c r="E20" s="349" t="s">
-        <v>327</v>
-      </c>
-      <c r="F20" s="348" t="s">
-        <v>328</v>
       </c>
       <c r="G20" s="350">
         <v>54768</v>
       </c>
       <c r="H20" s="348" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="I20" s="348" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="J20" s="348" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="21" spans="2:10" ht="32" customHeight="1">
       <c r="B21" s="348" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C21" s="348" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D21" s="348" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="E21" s="349" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="F21" s="348" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="G21" s="350">
         <v>42374</v>
       </c>
       <c r="H21" s="348" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="I21" s="348" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="J21" s="348" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="22" spans="2:10" ht="32" customHeight="1">
       <c r="B22" s="348" t="s">
+        <v>330</v>
+      </c>
+      <c r="C22" s="348" t="s">
+        <v>279</v>
+      </c>
+      <c r="D22" s="348" t="s">
+        <v>331</v>
+      </c>
+      <c r="E22" s="349" t="s">
         <v>332</v>
       </c>
-      <c r="C22" s="348" t="s">
-        <v>281</v>
-      </c>
-      <c r="D22" s="348" t="s">
-        <v>333</v>
-      </c>
-      <c r="E22" s="349" t="s">
-        <v>334</v>
-      </c>
       <c r="F22" s="348" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="G22" s="350">
         <v>42374</v>
       </c>
       <c r="H22" s="348" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="I22" s="348" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="J22" s="348" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="23" spans="2:10" ht="32" customHeight="1">
       <c r="B23" s="348" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C23" s="348" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D23" s="348" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="E23" s="349" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="F23" s="348" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="G23" s="350">
         <v>97714</v>
       </c>
       <c r="H23" s="348" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="I23" s="348" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="J23" s="348" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="24" spans="2:10" ht="32" customHeight="1">
       <c r="B24" s="348" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="C24" s="348" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D24" s="348" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="E24" s="349" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="F24" s="348" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="G24" s="350">
         <f>324010-SUM(G20:G23)</f>
         <v>86780</v>
       </c>
       <c r="H24" s="348" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="I24" s="348" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="J24" s="348" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="25" spans="2:10" ht="32" customHeight="1">
@@ -38047,8 +38064,8 @@
   </sheetPr>
   <dimension ref="A1:WVW57"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A17" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43:M43"/>
+    <sheetView showGridLines="0" topLeftCell="A7" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -38912,7 +38929,7 @@
     </row>
     <row r="15" spans="2:18" s="5" customFormat="1" ht="19" customHeight="1">
       <c r="C15" s="12" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="12"/>
@@ -38932,46 +38949,46 @@
       <c r="C18" s="370"/>
       <c r="D18" s="371"/>
       <c r="E18" s="506" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="F18" s="507"/>
       <c r="G18" s="507"/>
       <c r="H18" s="508"/>
       <c r="I18" s="444"/>
       <c r="J18" s="509" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="K18" s="510"/>
       <c r="L18" s="511"/>
     </row>
     <row r="19" spans="1:21" ht="57" customHeight="1">
       <c r="C19" s="372" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D19" s="373"/>
       <c r="E19" s="445" t="s">
+        <v>338</v>
+      </c>
+      <c r="F19" s="446" t="s">
+        <v>339</v>
+      </c>
+      <c r="G19" s="446" t="s">
         <v>340</v>
       </c>
-      <c r="F19" s="446" t="s">
+      <c r="H19" s="447" t="s">
         <v>341</v>
       </c>
-      <c r="G19" s="446" t="s">
+      <c r="I19" s="448" t="s">
         <v>342</v>
       </c>
-      <c r="H19" s="447" t="s">
+      <c r="J19" s="449" t="s">
         <v>343</v>
       </c>
-      <c r="I19" s="448" t="s">
+      <c r="K19" s="450" t="s">
         <v>344</v>
       </c>
-      <c r="J19" s="449" t="s">
+      <c r="L19" s="451" t="s">
         <v>345</v>
-      </c>
-      <c r="K19" s="450" t="s">
-        <v>346</v>
-      </c>
-      <c r="L19" s="451" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="20" spans="1:21" ht="15" customHeight="1">
@@ -38983,7 +39000,7 @@
       </c>
       <c r="F20" s="453">
         <f>D38</f>
-        <v>104000</v>
+        <v>156000</v>
       </c>
       <c r="G20" s="453">
         <f>H38</f>
@@ -38991,7 +39008,7 @@
       </c>
       <c r="H20" s="454">
         <f>E20-F20</f>
-        <v>185000</v>
+        <v>133000</v>
       </c>
       <c r="I20" s="455">
         <f>E20-I38</f>
@@ -39012,90 +39029,90 @@
     </row>
     <row r="22" spans="1:21" ht="15.75" customHeight="1">
       <c r="N22" s="360" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="P22" s="360"/>
       <c r="S22" s="409" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="T22" s="409" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="U22" s="441"/>
     </row>
     <row r="23" spans="1:21" s="356" customFormat="1" ht="20.25" customHeight="1">
       <c r="A23" s="512" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B23" s="514" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C23" s="515"/>
       <c r="D23" s="500" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="E23" s="502" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="F23" s="500"/>
       <c r="G23" s="500"/>
       <c r="H23" s="503"/>
       <c r="I23" s="504" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="J23" s="494" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="K23" s="495"/>
       <c r="L23" s="496"/>
       <c r="M23" s="497" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="N23" s="355"/>
       <c r="P23" s="499" t="s">
+        <v>355</v>
+      </c>
+      <c r="Q23" s="499" t="s">
+        <v>356</v>
+      </c>
+      <c r="S23" s="379" t="s">
         <v>357</v>
-      </c>
-      <c r="Q23" s="499" t="s">
-        <v>358</v>
-      </c>
-      <c r="S23" s="379" t="s">
-        <v>359</v>
       </c>
       <c r="T23" s="381" t="str">
         <f>IF(I38&lt;&gt;I39,"RED","Correct "&amp;I38&amp;" = "&amp;I39)</f>
         <v>Correct 289000 = 289000</v>
       </c>
       <c r="U23" s="516" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="24" spans="1:21" s="356" customFormat="1" ht="38.25" customHeight="1">
       <c r="A24" s="513"/>
       <c r="B24" s="428" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C24" s="394" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="D24" s="501"/>
       <c r="E24" s="392" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="F24" s="393" t="s">
+        <v>241</v>
+      </c>
+      <c r="G24" s="393" t="s">
         <v>243</v>
-      </c>
-      <c r="G24" s="393" t="s">
-        <v>245</v>
       </c>
       <c r="H24" s="394" t="s">
         <v>35</v>
       </c>
       <c r="I24" s="505"/>
       <c r="J24" s="392" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="K24" s="393" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="L24" s="394" t="s">
         <v>35</v>
@@ -39105,7 +39122,7 @@
       <c r="P24" s="499"/>
       <c r="Q24" s="499"/>
       <c r="S24" s="356" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="T24" s="382">
         <f>I39*0.3</f>
@@ -39238,7 +39255,7 @@
         <v>9910</v>
       </c>
       <c r="S26" s="380" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="T26" s="380">
         <f>LASTQUARTER</f>
@@ -39260,7 +39277,9 @@
       <c r="C27" s="385">
         <v>41455</v>
       </c>
-      <c r="D27" s="419"/>
+      <c r="D27" s="419">
+        <v>52000</v>
+      </c>
       <c r="E27" s="366">
         <v>71964</v>
       </c>
@@ -39297,7 +39316,7 @@
         <v>14817</v>
       </c>
       <c r="S27" s="380" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="T27" s="383">
         <f>I39*0.2</f>
@@ -39319,7 +39338,7 @@
       <c r="C28" s="385">
         <v>41547</v>
       </c>
-      <c r="D28" s="419"/>
+      <c r="D28" s="518"/>
       <c r="E28" s="366"/>
       <c r="F28" s="359"/>
       <c r="G28" s="359"/>
@@ -39409,7 +39428,7 @@
         <v>4927</v>
       </c>
       <c r="S29" s="380" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="T29" s="380" t="str">
         <f>IF(T23="RED","RED",IF(T25="RED","RED",IF(T28="AMBER","AMBER","GREEN")))</f>
@@ -39823,11 +39842,11 @@
     <row r="38" spans="1:21" ht="15.75" customHeight="1">
       <c r="B38" s="384"/>
       <c r="C38" s="424" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="D38" s="402">
         <f t="shared" ref="D38:M38" si="8">SUM(D25:D37)</f>
-        <v>104000</v>
+        <v>156000</v>
       </c>
       <c r="E38" s="406">
         <f t="shared" si="8"/>
@@ -39877,7 +39896,7 @@
     </row>
     <row r="39" spans="1:21">
       <c r="H39" s="426" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="I39" s="391">
         <f>E20</f>
@@ -39986,7 +40005,7 @@
     </row>
     <row r="46" spans="1:21" ht="26.25" hidden="1" customHeight="1">
       <c r="C46" s="427" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D46" s="386"/>
       <c r="E46" s="438">
@@ -40035,7 +40054,7 @@
     </row>
     <row r="47" spans="1:21" hidden="1">
       <c r="C47" s="426" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D47" s="389"/>
       <c r="E47" s="440">
@@ -40097,7 +40116,7 @@
     </row>
     <row r="48" spans="1:21" hidden="1">
       <c r="C48" s="426" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D48" s="389"/>
       <c r="E48" s="440">
@@ -40159,7 +40178,7 @@
     </row>
     <row r="49" spans="3:18" hidden="1">
       <c r="C49" s="426" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D49" s="389"/>
       <c r="E49" s="440">
@@ -40221,7 +40240,7 @@
     </row>
     <row r="50" spans="3:18" hidden="1">
       <c r="C50" s="426" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="D50" s="389"/>
       <c r="E50" s="440">
@@ -40283,7 +40302,7 @@
     </row>
     <row r="51" spans="3:18" ht="15" hidden="1" customHeight="1">
       <c r="C51" s="426" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D51" s="389"/>
       <c r="E51" s="440">
@@ -40294,12 +40313,12 @@
         <f>IF(F45&gt;LastDateReport,NA(),$D26+E51)</f>
         <v>104000</v>
       </c>
-      <c r="G51" s="440">
-        <f>IF(G45&gt;LastDateReport,NA(),D27+F51)</f>
-        <v>104000</v>
+      <c r="G51" s="440" t="e">
+        <f>IF(G45&gt;LastDateReport,NA(),#REF!+F51)</f>
+        <v>#REF!</v>
       </c>
       <c r="H51" s="440" t="e">
-        <f>IF(H45&gt;LastDateReport,NA(),D28+G51)</f>
+        <f>IF(H45&gt;LastDateReport,NA(),D27+G51)</f>
         <v>#N/A</v>
       </c>
       <c r="I51" s="440" t="e">
@@ -40340,12 +40359,12 @@
       </c>
       <c r="R51" s="440">
         <f>D38</f>
-        <v>104000</v>
+        <v>156000</v>
       </c>
     </row>
     <row r="52" spans="3:18" ht="26.25" hidden="1" customHeight="1">
       <c r="C52" s="427" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="D52" s="386"/>
       <c r="E52" s="438">
@@ -40394,7 +40413,7 @@
     </row>
     <row r="53" spans="3:18" hidden="1">
       <c r="C53" s="426" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D53" s="389"/>
       <c r="E53" s="440">
@@ -40456,7 +40475,7 @@
     </row>
     <row r="54" spans="3:18" hidden="1">
       <c r="C54" s="426" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="D54" s="389"/>
       <c r="E54" s="440">
@@ -40518,7 +40537,7 @@
     </row>
     <row r="55" spans="3:18" hidden="1">
       <c r="C55" s="389" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D55" s="389"/>
       <c r="E55" s="440">
@@ -40580,7 +40599,7 @@
     </row>
     <row r="56" spans="3:18" hidden="1">
       <c r="C56" s="389" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D56" s="389"/>
       <c r="E56" s="440">
@@ -41100,11 +41119,6 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27">
-    <cfRule type="expression" dxfId="75" priority="89">
-      <formula>$C25&gt;LastDateReport</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D28">
     <cfRule type="expression" dxfId="74" priority="90">
       <formula>$C25&gt;LastDateReport</formula>
     </cfRule>
@@ -41479,317 +41493,17 @@
       <formula>$C25&gt;LastDateReport</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="79">
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="Amount entered must be positive (no negative numbers.) No single amount can be greater than the Total EIF allocated to the project." sqref="J25">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="Amount entered must be positive (no negative numbers.) No single amount can be greater than the Total EIF allocated to the project." sqref="J26">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="Amount entered must be positive (no negative numbers.) No single amount can be greater than the Total EIF allocated to the project." sqref="J27">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="Amount entered must be positive (no negative numbers.) No single amount can be greater than the Total EIF allocated to the project." sqref="J28">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="Amount entered must be positive (no negative numbers.) No single amount can be greater than the Total EIF allocated to the project." sqref="J29">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="Amount entered must be positive (no negative numbers.) No single amount can be greater than the Total EIF allocated to the project." sqref="J30">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="Amount entered must be positive (no negative numbers.) No single amount can be greater than the Total EIF allocated to the project." sqref="J31">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="Amount entered must be positive (no negative numbers.) No single amount can be greater than the Total EIF allocated to the project." sqref="J32">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="Amount entered must be positive (no negative numbers.) No single amount can be greater than the Total EIF allocated to the project." sqref="J33">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="Amount entered must be positive (no negative numbers.) No single amount can be greater than the Total EIF allocated to the project." sqref="J34">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="Amount entered must be positive (no negative numbers.) No single amount can be greater than the Total EIF allocated to the project." sqref="J35">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="Amount entered must be positive (no negative numbers.) No single amount can be greater than the Total EIF allocated to the project." sqref="J36">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="Amount entered must be positive (no negative numbers.) No single amount can be greater than the Total EIF allocated to the project." sqref="J37">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="Amount entered must be positive (no negative numbers.) No single amount can be greater than the Total EIF allocated to the project." sqref="K25">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="Amount entered must be positive (no negative numbers.) No single amount can be greater than the Total EIF allocated to the project." sqref="K26">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="Amount entered must be positive (no negative numbers.) No single amount can be greater than the Total EIF allocated to the project." sqref="K27">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="Amount entered must be positive (no negative numbers.) No single amount can be greater than the Total EIF allocated to the project." sqref="K28">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="Amount entered must be positive (no negative numbers.) No single amount can be greater than the Total EIF allocated to the project." sqref="K29">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="Amount entered must be positive (no negative numbers.) No single amount can be greater than the Total EIF allocated to the project." sqref="K30">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="Amount entered must be positive (no negative numbers.) No single amount can be greater than the Total EIF allocated to the project." sqref="K31">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="Amount entered must be positive (no negative numbers.) No single amount can be greater than the Total EIF allocated to the project." sqref="K32">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="Amount entered must be positive (no negative numbers.) No single amount can be greater than the Total EIF allocated to the project." sqref="K33">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="Amount entered must be positive (no negative numbers.) No single amount can be greater than the Total EIF allocated to the project." sqref="K34">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="Amount entered must be positive (no negative numbers.) No single amount can be greater than the Total EIF allocated to the project." sqref="K35">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="Amount entered must be positive (no negative numbers.) No single amount can be greater than the Total EIF allocated to the project." sqref="K36">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="Amount entered must be positive (no negative numbers.) No single amount can be greater than the Total EIF allocated to the project." sqref="K37">
+  <dataValidations count="4">
+    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="Amount entered must be positive (no negative numbers.) No single amount can be greater than the Total EIF allocated to the project." sqref="J25:K37">
       <formula1>0</formula1>
       <formula2>TOTALEIF</formula2>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="TOTAL to equal EIF Total" prompt="The Project Manager is to modify the projected cash flow as appropriate, ensuring ACTUAL spend is listed where available, and best estimate is used for future spend. The total should equal the EIF allocated. The total will be red if it is not equal to EIF" sqref="I38"/>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="Amount entered must be positive (no negative numbers.) No single amount can be greater than the Total EIF allocated to the project." promptTitle="Show ACTUAL where available" prompt="If the cell is red, please update it with the actual value for period shown in the cell to the left._x000a_HINT: You can move this box so it does not obscure the column, or click away from the column to hide it." sqref="I25">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="Amount entered must be positive (no negative numbers.) No single amount can be greater than the Total EIF allocated to the project." promptTitle="Show ACTUAL where available" prompt="If the cell is red, please update it with the actual value for period shown in the cell to the left._x000a_HINT: You can move this box so it does not obscure the column, or click away from the column to hide it." sqref="I25:I37">
       <formula1>0</formula1>
       <formula2>TOTALEIF</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="Amount entered must be positive (no negative numbers.) No single amount can be greater than the Total EIF allocated to the project." promptTitle="Show ACTUAL where available" prompt="If the cell is red, please update it with the actual value for period shown in the cell to the left._x000a_HINT: You can move this box so it does not obscure the column, or click away from the column to hide it." sqref="I26">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="Amount entered must be positive (no negative numbers.) No single amount can be greater than the Total EIF allocated to the project." promptTitle="Show ACTUAL where available" prompt="If the cell is red, please update it with the actual value for period shown in the cell to the left._x000a_HINT: You can move this box so it does not obscure the column, or click away from the column to hide it." sqref="I27">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="Amount entered must be positive (no negative numbers.) No single amount can be greater than the Total EIF allocated to the project." promptTitle="Show ACTUAL where available" prompt="If the cell is red, please update it with the actual value for period shown in the cell to the left._x000a_HINT: You can move this box so it does not obscure the column, or click away from the column to hide it." sqref="I28">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="Amount entered must be positive (no negative numbers.) No single amount can be greater than the Total EIF allocated to the project." promptTitle="Show ACTUAL where available" prompt="If the cell is red, please update it with the actual value for period shown in the cell to the left._x000a_HINT: You can move this box so it does not obscure the column, or click away from the column to hide it." sqref="I29">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="Amount entered must be positive (no negative numbers.) No single amount can be greater than the Total EIF allocated to the project." promptTitle="Show ACTUAL where available" prompt="If the cell is red, please update it with the actual value for period shown in the cell to the left._x000a_HINT: You can move this box so it does not obscure the column, or click away from the column to hide it." sqref="I30">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="Amount entered must be positive (no negative numbers.) No single amount can be greater than the Total EIF allocated to the project." promptTitle="Show ACTUAL where available" prompt="If the cell is red, please update it with the actual value for period shown in the cell to the left._x000a_HINT: You can move this box so it does not obscure the column, or click away from the column to hide it." sqref="I31">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="Amount entered must be positive (no negative numbers.) No single amount can be greater than the Total EIF allocated to the project." promptTitle="Show ACTUAL where available" prompt="If the cell is red, please update it with the actual value for period shown in the cell to the left._x000a_HINT: You can move this box so it does not obscure the column, or click away from the column to hide it." sqref="I32">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="Amount entered must be positive (no negative numbers.) No single amount can be greater than the Total EIF allocated to the project." promptTitle="Show ACTUAL where available" prompt="If the cell is red, please update it with the actual value for period shown in the cell to the left._x000a_HINT: You can move this box so it does not obscure the column, or click away from the column to hide it." sqref="I33">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="Amount entered must be positive (no negative numbers.) No single amount can be greater than the Total EIF allocated to the project." promptTitle="Show ACTUAL where available" prompt="If the cell is red, please update it with the actual value for period shown in the cell to the left._x000a_HINT: You can move this box so it does not obscure the column, or click away from the column to hide it." sqref="I34">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="Amount entered must be positive (no negative numbers.) No single amount can be greater than the Total EIF allocated to the project." promptTitle="Show ACTUAL where available" prompt="If the cell is red, please update it with the actual value for period shown in the cell to the left._x000a_HINT: You can move this box so it does not obscure the column, or click away from the column to hide it." sqref="I35">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="Amount entered must be positive (no negative numbers.) No single amount can be greater than the Total EIF allocated to the project." promptTitle="Show ACTUAL where available" prompt="If the cell is red, please update it with the actual value for period shown in the cell to the left._x000a_HINT: You can move this box so it does not obscure the column, or click away from the column to hide it." sqref="I36">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="Amount entered must be positive (no negative numbers.) No single amount can be greater than the Total EIF allocated to the project." promptTitle="Show ACTUAL where available" prompt="If the cell is red, please update it with the actual value for period shown in the cell to the left._x000a_HINT: You can move this box so it does not obscure the column, or click away from the column to hide it." sqref="I37">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="The amount entered must be positive (no negative numbers), and must not be greater than the total EIF allocated to the project." sqref="E25">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="The amount entered must be positive (no negative numbers), and must not be greater than the total EIF allocated to the project." sqref="E26">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="The amount entered must be positive (no negative numbers), and must not be greater than the total EIF allocated to the project." sqref="E27">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="The amount entered must be positive (no negative numbers), and must not be greater than the total EIF allocated to the project." sqref="E28">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="The amount entered must be positive (no negative numbers), and must not be greater than the total EIF allocated to the project." sqref="E29">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="The amount entered must be positive (no negative numbers), and must not be greater than the total EIF allocated to the project." sqref="E30">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="The amount entered must be positive (no negative numbers), and must not be greater than the total EIF allocated to the project." sqref="E31">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="The amount entered must be positive (no negative numbers), and must not be greater than the total EIF allocated to the project." sqref="E32">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="The amount entered must be positive (no negative numbers), and must not be greater than the total EIF allocated to the project." sqref="E33">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="The amount entered must be positive (no negative numbers), and must not be greater than the total EIF allocated to the project." sqref="E34">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="The amount entered must be positive (no negative numbers), and must not be greater than the total EIF allocated to the project." sqref="E35">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="The amount entered must be positive (no negative numbers), and must not be greater than the total EIF allocated to the project." sqref="E36">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="The amount entered must be positive (no negative numbers), and must not be greater than the total EIF allocated to the project." sqref="E37">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="The amount entered must be positive (no negative numbers), and must not be greater than the total EIF allocated to the project." sqref="F25">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="The amount entered must be positive (no negative numbers), and must not be greater than the total EIF allocated to the project." sqref="F26">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="The amount entered must be positive (no negative numbers), and must not be greater than the total EIF allocated to the project." sqref="F27">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="The amount entered must be positive (no negative numbers), and must not be greater than the total EIF allocated to the project." sqref="F28">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="The amount entered must be positive (no negative numbers), and must not be greater than the total EIF allocated to the project." sqref="F29">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="The amount entered must be positive (no negative numbers), and must not be greater than the total EIF allocated to the project." sqref="F30">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="The amount entered must be positive (no negative numbers), and must not be greater than the total EIF allocated to the project." sqref="F31">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="The amount entered must be positive (no negative numbers), and must not be greater than the total EIF allocated to the project." sqref="F32">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="The amount entered must be positive (no negative numbers), and must not be greater than the total EIF allocated to the project." sqref="F33">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="The amount entered must be positive (no negative numbers), and must not be greater than the total EIF allocated to the project." sqref="F34">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="The amount entered must be positive (no negative numbers), and must not be greater than the total EIF allocated to the project." sqref="F35">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="The amount entered must be positive (no negative numbers), and must not be greater than the total EIF allocated to the project." sqref="F36">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="The amount entered must be positive (no negative numbers), and must not be greater than the total EIF allocated to the project." sqref="F37">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="The amount entered must be positive (no negative numbers), and must not be greater than the total EIF allocated to the project." sqref="G25">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="The amount entered must be positive (no negative numbers), and must not be greater than the total EIF allocated to the project." sqref="G26">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="The amount entered must be positive (no negative numbers), and must not be greater than the total EIF allocated to the project." sqref="G27">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="The amount entered must be positive (no negative numbers), and must not be greater than the total EIF allocated to the project." sqref="G28">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="The amount entered must be positive (no negative numbers), and must not be greater than the total EIF allocated to the project." sqref="G29">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="The amount entered must be positive (no negative numbers), and must not be greater than the total EIF allocated to the project." sqref="G30">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="The amount entered must be positive (no negative numbers), and must not be greater than the total EIF allocated to the project." sqref="G31">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="The amount entered must be positive (no negative numbers), and must not be greater than the total EIF allocated to the project." sqref="G32">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="The amount entered must be positive (no negative numbers), and must not be greater than the total EIF allocated to the project." sqref="G33">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="The amount entered must be positive (no negative numbers), and must not be greater than the total EIF allocated to the project." sqref="G34">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="The amount entered must be positive (no negative numbers), and must not be greater than the total EIF allocated to the project." sqref="G35">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="The amount entered must be positive (no negative numbers), and must not be greater than the total EIF allocated to the project." sqref="G36">
-      <formula1>0</formula1>
-      <formula2>TOTALEIF</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="The amount entered must be positive (no negative numbers), and must not be greater than the total EIF allocated to the project." sqref="G37">
+    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="AMOUNT ERROR" error="The amount entered must be positive (no negative numbers), and must not be greater than the total EIF allocated to the project." sqref="E25:G37">
       <formula1>0</formula1>
       <formula2>TOTALEIF</formula2>
     </dataValidation>
@@ -41827,8 +41541,8 @@
   </sheetPr>
   <dimension ref="A1:R58"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView showGridLines="0" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -42598,7 +42312,7 @@
       </c>
       <c r="L28" s="194"/>
       <c r="M28" s="315" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="N28" s="162" t="str">
         <f t="shared" si="1"/>
@@ -42646,7 +42360,7 @@
       </c>
       <c r="L29" s="194"/>
       <c r="M29" s="315" t="s">
-        <v>89</v>
+        <v>394</v>
       </c>
       <c r="N29" s="162" t="str">
         <f t="shared" si="1"/>
@@ -42669,10 +42383,10 @@
         <v>12</v>
       </c>
       <c r="D30" s="323" t="s">
+        <v>89</v>
+      </c>
+      <c r="E30" s="323" t="s">
         <v>90</v>
-      </c>
-      <c r="E30" s="323" t="s">
-        <v>91</v>
       </c>
       <c r="F30" s="191">
         <v>41243</v>
@@ -42694,7 +42408,7 @@
       <c r="K30" s="193"/>
       <c r="L30" s="194"/>
       <c r="M30" s="315" t="s">
-        <v>382</v>
+        <v>395</v>
       </c>
       <c r="N30" s="162" t="str">
         <f t="shared" si="1"/>
@@ -42717,10 +42431,10 @@
         <v>13</v>
       </c>
       <c r="D31" s="323" t="s">
+        <v>91</v>
+      </c>
+      <c r="E31" s="323" t="s">
         <v>92</v>
-      </c>
-      <c r="E31" s="323" t="s">
-        <v>93</v>
       </c>
       <c r="F31" s="191">
         <v>41258</v>
@@ -42741,7 +42455,7 @@
       </c>
       <c r="L31" s="194"/>
       <c r="M31" s="315" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="N31" s="162" t="str">
         <f t="shared" si="1"/>
@@ -42766,10 +42480,10 @@
         <v>14</v>
       </c>
       <c r="D32" s="323" t="s">
+        <v>93</v>
+      </c>
+      <c r="E32" s="323" t="s">
         <v>94</v>
-      </c>
-      <c r="E32" s="323" t="s">
-        <v>95</v>
       </c>
       <c r="F32" s="191">
         <v>41258</v>
@@ -42790,7 +42504,7 @@
       </c>
       <c r="L32" s="194"/>
       <c r="M32" s="315" t="s">
-        <v>390</v>
+        <v>396</v>
       </c>
       <c r="N32" s="162" t="str">
         <f t="shared" si="1"/>
@@ -42815,10 +42529,10 @@
         <v>15</v>
       </c>
       <c r="D33" s="323" t="s">
+        <v>95</v>
+      </c>
+      <c r="E33" s="323" t="s">
         <v>96</v>
-      </c>
-      <c r="E33" s="323" t="s">
-        <v>97</v>
       </c>
       <c r="F33" s="191">
         <v>41333</v>
@@ -42840,7 +42554,7 @@
       </c>
       <c r="L33" s="194"/>
       <c r="M33" s="315" t="s">
-        <v>98</v>
+        <v>397</v>
       </c>
       <c r="N33" s="162" t="str">
         <f t="shared" si="1"/>
@@ -42865,10 +42579,10 @@
         <v>16</v>
       </c>
       <c r="D34" s="323" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E34" s="323" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F34" s="191">
         <v>41334</v>
@@ -42911,10 +42625,10 @@
         <v>17</v>
       </c>
       <c r="D35" s="323" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E35" s="323" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F35" s="191">
         <v>41600</v>
@@ -42957,10 +42671,10 @@
         <v>18</v>
       </c>
       <c r="D36" s="323" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E36" s="323" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F36" s="191">
         <v>41820</v>
@@ -43002,7 +42716,7 @@
       <c r="G37" s="66"/>
       <c r="H37" s="66"/>
       <c r="I37" s="26" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J37" s="66"/>
       <c r="K37" s="66"/>
@@ -43010,7 +42724,7 @@
       <c r="M37" s="66"/>
       <c r="N37" s="66"/>
       <c r="O37" s="226" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="P37" s="226" t="str">
         <f>IF(COUNTIF(P19:P36,"RED")&gt;0,"RED",IF(COUNTIF(P19:P36,"AMBER")&gt;0,"AMBER","GREEN"))</f>
@@ -44273,7 +43987,7 @@
     <row r="15" spans="1:18" ht="20" customHeight="1">
       <c r="A15" s="65"/>
       <c r="B15" s="47" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C15" s="30"/>
       <c r="D15" s="30"/>
@@ -44300,7 +44014,7 @@
     <row r="16" spans="1:18" ht="17" customHeight="1">
       <c r="A16" s="65"/>
       <c r="B16" s="477" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C16" s="477"/>
       <c r="D16" s="477"/>
@@ -44338,29 +44052,29 @@
     </row>
     <row r="18" spans="1:18" ht="47.25" customHeight="1">
       <c r="B18" s="74" t="s">
+        <v>107</v>
+      </c>
+      <c r="C18" s="75" t="s">
+        <v>108</v>
+      </c>
+      <c r="D18" s="75" t="s">
         <v>109</v>
       </c>
-      <c r="C18" s="75" t="s">
+      <c r="E18" s="75" t="s">
         <v>110</v>
       </c>
-      <c r="D18" s="75" t="s">
+      <c r="F18" s="76" t="s">
         <v>111</v>
-      </c>
-      <c r="E18" s="75" t="s">
-        <v>112</v>
-      </c>
-      <c r="F18" s="76" t="s">
-        <v>113</v>
       </c>
       <c r="G18" s="180"/>
       <c r="H18" s="181" t="s">
+        <v>112</v>
+      </c>
+      <c r="I18" s="181" t="s">
+        <v>113</v>
+      </c>
+      <c r="J18" s="76" t="s">
         <v>114</v>
-      </c>
-      <c r="I18" s="181" t="s">
-        <v>115</v>
-      </c>
-      <c r="J18" s="76" t="s">
-        <v>116</v>
       </c>
       <c r="K18" s="65"/>
       <c r="L18" s="65"/>
@@ -44613,17 +44327,17 @@
     </row>
     <row r="28" spans="1:18" ht="15" customHeight="1">
       <c r="B28" s="84" t="s">
+        <v>115</v>
+      </c>
+      <c r="C28" s="85" t="s">
+        <v>116</v>
+      </c>
+      <c r="D28" s="84" t="s">
         <v>117</v>
-      </c>
-      <c r="C28" s="85" t="s">
-        <v>118</v>
-      </c>
-      <c r="D28" s="84" t="s">
-        <v>119</v>
       </c>
       <c r="E28" s="476"/>
       <c r="F28" s="84" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G28" s="86"/>
       <c r="H28" s="86"/>
@@ -45108,7 +44822,7 @@
   <dimension ref="A1:O51"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="B19" sqref="B19:E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -45265,7 +44979,7 @@
     <row r="15" spans="1:15" ht="19" customHeight="1">
       <c r="A15" s="65"/>
       <c r="B15" s="12" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C15" s="30"/>
       <c r="D15" s="30" t="s">
@@ -45289,7 +45003,7 @@
     <row r="16" spans="1:15" ht="16" customHeight="1">
       <c r="A16" s="5"/>
       <c r="B16" s="477" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C16" s="477"/>
       <c r="D16" s="477"/>
@@ -45323,16 +45037,16 @@
     </row>
     <row r="18" spans="1:15" ht="27" customHeight="1">
       <c r="B18" s="43" t="s">
+        <v>121</v>
+      </c>
+      <c r="C18" s="44" t="s">
+        <v>122</v>
+      </c>
+      <c r="D18" s="44" t="s">
         <v>123</v>
       </c>
-      <c r="C18" s="44" t="s">
+      <c r="E18" s="45" t="s">
         <v>124</v>
-      </c>
-      <c r="D18" s="44" t="s">
-        <v>125</v>
-      </c>
-      <c r="E18" s="45" t="s">
-        <v>126</v>
       </c>
       <c r="F18" s="77"/>
       <c r="G18" s="4"/>
@@ -45350,16 +45064,16 @@
         <v>48</v>
       </c>
       <c r="B19" s="302" t="s">
+        <v>125</v>
+      </c>
+      <c r="C19" s="416" t="s">
+        <v>126</v>
+      </c>
+      <c r="D19" s="304" t="s">
+        <v>388</v>
+      </c>
+      <c r="E19" s="410" t="s">
         <v>127</v>
-      </c>
-      <c r="C19" s="416" t="s">
-        <v>128</v>
-      </c>
-      <c r="D19" s="304" t="s">
-        <v>392</v>
-      </c>
-      <c r="E19" s="410" t="s">
-        <v>129</v>
       </c>
       <c r="F19" s="93"/>
       <c r="G19" s="48" t="str">
@@ -45380,13 +45094,13 @@
         <v>1</v>
       </c>
       <c r="C20" s="303" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D20" s="304" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="E20" s="410" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F20" s="93"/>
       <c r="G20" s="48" t="str">
@@ -45407,13 +45121,13 @@
         <v>2</v>
       </c>
       <c r="C21" s="303" t="s">
+        <v>129</v>
+      </c>
+      <c r="D21" s="304" t="s">
+        <v>130</v>
+      </c>
+      <c r="E21" s="410" t="s">
         <v>131</v>
-      </c>
-      <c r="D21" s="304" t="s">
-        <v>132</v>
-      </c>
-      <c r="E21" s="410" t="s">
-        <v>133</v>
       </c>
       <c r="F21" s="93"/>
       <c r="G21" s="48" t="str">
@@ -45434,13 +45148,13 @@
         <v>3</v>
       </c>
       <c r="C22" s="303" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D22" s="304" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="E22" s="410" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F22" s="93"/>
       <c r="G22" s="48" t="str">
@@ -45461,13 +45175,13 @@
         <v>4</v>
       </c>
       <c r="C23" s="306" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D23" s="307" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E23" s="411" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F23" s="93"/>
       <c r="G23" s="48" t="str">
@@ -46136,7 +45850,7 @@
     <row r="15" spans="1:28" s="4" customFormat="1" ht="19" customHeight="1">
       <c r="A15" s="65"/>
       <c r="B15" s="12" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C15" s="12"/>
       <c r="D15" s="12"/>
@@ -46153,7 +45867,7 @@
       <c r="J15" s="94"/>
       <c r="K15" s="94"/>
       <c r="L15" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="M15" s="1"/>
       <c r="N15" s="1">
@@ -46165,7 +45879,7 @@
     <row r="16" spans="1:28" s="4" customFormat="1" ht="16" customHeight="1">
       <c r="A16" s="65"/>
       <c r="B16" s="46" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C16" s="186"/>
       <c r="D16" s="46"/>
@@ -46177,7 +45891,7 @@
       <c r="J16" s="91"/>
       <c r="K16" s="91"/>
       <c r="L16" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="M16" s="1"/>
       <c r="N16" s="1" t="str">
@@ -46198,7 +45912,7 @@
       <c r="J17" s="63"/>
       <c r="K17" s="63"/>
       <c r="L17" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="M17" s="1"/>
       <c r="N17" s="1">
@@ -46209,32 +45923,32 @@
     </row>
     <row r="18" spans="1:28" s="4" customFormat="1" ht="57.75" customHeight="1">
       <c r="B18" s="49" t="s">
+        <v>140</v>
+      </c>
+      <c r="C18" s="198" t="s">
+        <v>141</v>
+      </c>
+      <c r="D18" s="50" t="s">
         <v>142</v>
       </c>
-      <c r="C18" s="198" t="s">
+      <c r="E18" s="50" t="s">
         <v>143</v>
       </c>
-      <c r="D18" s="50" t="s">
+      <c r="F18" s="50" t="s">
         <v>144</v>
       </c>
-      <c r="E18" s="50" t="s">
+      <c r="G18" s="50" t="s">
+        <v>114</v>
+      </c>
+      <c r="H18" s="50" t="s">
         <v>145</v>
       </c>
-      <c r="F18" s="50" t="s">
+      <c r="I18" s="51" t="s">
         <v>146</v>
-      </c>
-      <c r="G18" s="50" t="s">
-        <v>116</v>
-      </c>
-      <c r="H18" s="50" t="s">
-        <v>147</v>
-      </c>
-      <c r="I18" s="51" t="s">
-        <v>148</v>
       </c>
       <c r="J18" s="95"/>
       <c r="K18" s="96" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="AB18" s="2"/>
     </row>
@@ -46243,10 +45957,10 @@
         <v>48</v>
       </c>
       <c r="B19" s="324" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C19" s="325" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D19" s="326">
         <v>0</v>
@@ -46530,13 +46244,13 @@
       <c r="E28" s="33"/>
       <c r="F28" s="33"/>
       <c r="G28" s="36" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H28" s="29"/>
       <c r="I28" s="33"/>
       <c r="J28" s="63"/>
       <c r="K28" s="99" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="M28" s="32" t="str">
         <f>IF(COUNTIF(M19:M27,"RED")&gt;0,"RED",IF(COUNTIF(M19:M27,"AMBER")&gt;0,"AMBER","GREEN"))</f>
@@ -50927,7 +50641,7 @@
   </sheetPr>
   <dimension ref="A1:O60"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A19" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
@@ -51076,7 +50790,7 @@
     </row>
     <row r="15" spans="1:15" ht="19" customHeight="1">
       <c r="B15" s="94" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C15" s="94"/>
       <c r="D15" s="94"/>
@@ -51085,7 +50799,7 @@
     </row>
     <row r="16" spans="1:15" ht="16" customHeight="1">
       <c r="B16" s="477" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C16" s="477"/>
       <c r="D16" s="477"/>
@@ -51101,22 +50815,22 @@
     </row>
     <row r="18" spans="1:7" ht="44" customHeight="1">
       <c r="B18" s="227" t="s">
+        <v>153</v>
+      </c>
+      <c r="C18" s="227" t="s">
+        <v>154</v>
+      </c>
+      <c r="D18" s="227" t="s">
         <v>155</v>
       </c>
-      <c r="C18" s="227" t="s">
+      <c r="E18" s="227" t="s">
         <v>156</v>
-      </c>
-      <c r="D18" s="227" t="s">
-        <v>157</v>
-      </c>
-      <c r="E18" s="227" t="s">
-        <v>158</v>
       </c>
       <c r="F18" s="227" t="s">
         <v>33</v>
       </c>
       <c r="G18" s="214" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="42" customHeight="1">
@@ -51124,87 +50838,87 @@
         <v>48</v>
       </c>
       <c r="B19" s="281" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C19" s="281" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D19" s="282">
         <v>41000</v>
       </c>
       <c r="E19" s="281" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F19" s="461" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="G19" s="96"/>
     </row>
     <row r="20" spans="1:7" ht="44" customHeight="1">
       <c r="B20" s="281" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C20" s="281" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D20" s="282">
         <v>41122</v>
       </c>
       <c r="E20" s="281" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F20" s="461"/>
       <c r="G20" s="96"/>
     </row>
     <row r="21" spans="1:7" ht="44" customHeight="1">
       <c r="B21" s="281" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C21" s="281" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D21" s="282"/>
       <c r="E21" s="281" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F21" s="461" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G21" s="96"/>
     </row>
     <row r="22" spans="1:7" ht="44" customHeight="1">
       <c r="B22" s="281" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C22" s="281" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D22" s="282">
         <v>41122</v>
       </c>
       <c r="E22" s="281" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F22" s="461" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G22" s="96"/>
     </row>
     <row r="23" spans="1:7" ht="42" customHeight="1">
       <c r="B23" s="281" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C23" s="281" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D23" s="282">
         <v>41091</v>
       </c>
       <c r="E23" s="281" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F23" s="461" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G23" s="96"/>
     </row>
@@ -51546,8 +51260,8 @@
   </sheetPr>
   <dimension ref="A1:R50"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="R20" sqref="R20"/>
+    <sheetView showGridLines="0" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="R28" sqref="R26:R28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -51773,7 +51487,7 @@
     </row>
     <row r="15" spans="1:18" ht="19" customHeight="1">
       <c r="B15" s="12" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C15" s="12"/>
       <c r="D15" s="12"/>
@@ -51785,7 +51499,7 @@
     </row>
     <row r="16" spans="1:18" ht="16" customHeight="1">
       <c r="B16" s="477" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C16" s="477"/>
       <c r="D16" s="477"/>
@@ -51813,81 +51527,81 @@
       <c r="E18" s="137"/>
       <c r="F18" s="137"/>
       <c r="G18" s="481" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H18" s="482"/>
       <c r="I18" s="481" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J18" s="482"/>
       <c r="K18" s="481" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="L18" s="482"/>
       <c r="M18" s="479" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="N18" s="480"/>
       <c r="O18" s="479" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="P18" s="480"/>
       <c r="Q18" s="479" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="R18" s="480"/>
     </row>
     <row r="19" spans="2:18" ht="32" customHeight="1">
       <c r="B19" s="139" t="s">
+        <v>182</v>
+      </c>
+      <c r="C19" s="140" t="s">
+        <v>183</v>
+      </c>
+      <c r="D19" s="140" t="s">
         <v>184</v>
       </c>
-      <c r="C19" s="140" t="s">
+      <c r="E19" s="142" t="s">
         <v>185</v>
       </c>
-      <c r="D19" s="140" t="s">
+      <c r="F19" s="217" t="s">
         <v>186</v>
       </c>
-      <c r="E19" s="142" t="s">
+      <c r="G19" s="216" t="s">
         <v>187</v>
       </c>
-      <c r="F19" s="217" t="s">
+      <c r="H19" s="144" t="s">
         <v>188</v>
       </c>
-      <c r="G19" s="216" t="s">
-        <v>189</v>
-      </c>
-      <c r="H19" s="144" t="s">
-        <v>190</v>
-      </c>
       <c r="I19" s="143" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="J19" s="144" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="K19" s="143" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="L19" s="144" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="M19" s="143" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="N19" s="144" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="O19" s="143" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="P19" s="144" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="Q19" s="143" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="R19" s="144" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="20" spans="2:18" s="4" customFormat="1" ht="28" customHeight="1">
@@ -51904,19 +51618,19 @@
         <v>41044</v>
       </c>
       <c r="F20" s="286" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G20" s="287">
         <v>15</v>
       </c>
       <c r="H20" s="146">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="I20" s="145" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="J20" s="147" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="K20" s="145"/>
       <c r="L20" s="147"/>
@@ -51931,7 +51645,9 @@
       <c r="Q20" s="145">
         <v>32500</v>
       </c>
-      <c r="R20" s="147"/>
+      <c r="R20" s="147">
+        <v>45000</v>
+      </c>
     </row>
     <row r="21" spans="2:18" ht="28" customHeight="1">
       <c r="B21" s="283">
@@ -51947,19 +51663,19 @@
         <v>41136</v>
       </c>
       <c r="F21" s="286" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="G21" s="287">
         <v>0</v>
       </c>
       <c r="H21" s="146">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="I21" s="145" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="J21" s="148" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="K21" s="145"/>
       <c r="L21" s="147"/>
@@ -51984,7 +51700,7 @@
         <v>41167</v>
       </c>
       <c r="F22" s="286" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="G22" s="287">
         <v>0</v>
@@ -51993,10 +51709,10 @@
         <v>4</v>
       </c>
       <c r="I22" s="145" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="J22" s="148" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="K22" s="145"/>
       <c r="L22" s="147"/>
@@ -52021,19 +51737,19 @@
         <v>41167</v>
       </c>
       <c r="F23" s="286" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G23" s="287">
         <v>9</v>
       </c>
       <c r="H23" s="147">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="I23" s="145" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="J23" s="148" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="K23" s="145"/>
       <c r="L23" s="147">
@@ -52068,15 +51784,15 @@
         <v>41212</v>
       </c>
       <c r="F24" s="286" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G24" s="287"/>
       <c r="H24" s="147">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="I24" s="145"/>
       <c r="J24" s="148" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="K24" s="145"/>
       <c r="L24" s="147"/>
@@ -52101,7 +51817,7 @@
         <v>41228</v>
       </c>
       <c r="F25" s="286" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G25" s="287"/>
       <c r="H25" s="147"/>
@@ -52121,7 +51837,7 @@
         <v>7</v>
       </c>
       <c r="C26" s="283" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D26" s="284">
         <v>41258</v>
@@ -52130,15 +51846,15 @@
         <v>41304</v>
       </c>
       <c r="F26" s="286" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="G26" s="287"/>
       <c r="H26" s="147">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="I26" s="145"/>
       <c r="J26" s="148" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="K26" s="145"/>
       <c r="L26" s="147"/>
@@ -52154,7 +51870,7 @@
         <v>8</v>
       </c>
       <c r="C27" s="283" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D27" s="284">
         <v>41258</v>
@@ -52163,17 +51879,17 @@
         <v>41304</v>
       </c>
       <c r="F27" s="286" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G27" s="287"/>
       <c r="H27" s="147">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="I27" s="145" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="J27" s="148" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="K27" s="145"/>
       <c r="L27" s="147"/>
@@ -52189,7 +51905,7 @@
         <v>9</v>
       </c>
       <c r="C28" s="283" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D28" s="284">
         <v>41333</v>
@@ -52198,7 +51914,7 @@
         <v>41363</v>
       </c>
       <c r="F28" s="286" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="G28" s="287"/>
       <c r="H28" s="147"/>
@@ -52311,7 +52027,7 @@
     <row r="34" spans="2:18" ht="15" customHeight="1"/>
     <row r="35" spans="2:18" ht="46" customHeight="1">
       <c r="C35" s="158" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D35" s="159"/>
     </row>
@@ -52320,7 +52036,7 @@
     </row>
     <row r="37" spans="2:18">
       <c r="B37" s="18" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="38" spans="2:18" ht="14" customHeight="1">
@@ -52337,27 +52053,27 @@
     <row r="40" spans="2:18">
       <c r="B40" s="17"/>
       <c r="C40" s="460" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="41" spans="2:18">
       <c r="C41" s="460" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="42" spans="2:18">
       <c r="C42" s="460" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="43" spans="2:18">
       <c r="C43" s="460" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="44" spans="2:18">
       <c r="C44" s="460" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="O44" s="4"/>
       <c r="P44" s="5"/>
@@ -52366,7 +52082,7 @@
     </row>
     <row r="45" spans="2:18" ht="15" customHeight="1">
       <c r="C45" s="460" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="P45" s="5"/>
     </row>
@@ -52563,7 +52279,7 @@
   <dimension ref="A1:O55"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -52734,7 +52450,7 @@
     <row r="15" spans="1:15" ht="19" customHeight="1">
       <c r="A15" s="65"/>
       <c r="B15" s="12" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C15" s="12"/>
       <c r="D15" s="12"/>
@@ -52755,20 +52471,20 @@
     <row r="17" spans="1:7" ht="15" customHeight="1">
       <c r="A17" s="65"/>
       <c r="B17" s="53" t="s">
+        <v>208</v>
+      </c>
+      <c r="C17" s="54" t="s">
+        <v>209</v>
+      </c>
+      <c r="D17" s="218" t="s">
         <v>210</v>
       </c>
-      <c r="C17" s="54" t="s">
+      <c r="E17" s="55" t="s">
         <v>211</v>
-      </c>
-      <c r="D17" s="218" t="s">
-        <v>212</v>
-      </c>
-      <c r="E17" s="55" t="s">
-        <v>213</v>
       </c>
       <c r="F17" s="103"/>
       <c r="G17" s="56" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="28" customHeight="1">
@@ -52776,16 +52492,16 @@
         <v>48</v>
       </c>
       <c r="B18" s="290" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="C18" s="296" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D18" s="275" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E18" s="299" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="F18" s="101"/>
       <c r="G18" s="57" t="str">
@@ -52796,13 +52512,13 @@
     <row r="19" spans="1:7" ht="28" customHeight="1">
       <c r="A19" s="65"/>
       <c r="B19" s="290" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C19" s="296" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D19" s="275" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E19" s="298"/>
       <c r="F19" s="101"/>
@@ -52814,13 +52530,13 @@
     <row r="20" spans="1:7" s="5" customFormat="1" ht="28" customHeight="1">
       <c r="A20" s="65"/>
       <c r="B20" s="290" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="C20" s="296" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D20" s="275" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E20" s="298"/>
       <c r="F20" s="101"/>
@@ -52831,16 +52547,16 @@
     </row>
     <row r="21" spans="1:7" s="5" customFormat="1" ht="28" customHeight="1">
       <c r="B21" s="290" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="C21" s="296" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D21" s="275" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E21" s="299" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="F21" s="101"/>
       <c r="G21" s="57" t="str">
@@ -52850,13 +52566,13 @@
     </row>
     <row r="22" spans="1:7" s="5" customFormat="1" ht="28" customHeight="1">
       <c r="B22" s="308" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="C22" s="461" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D22" s="275" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E22" s="298"/>
       <c r="F22" s="101"/>
@@ -52869,7 +52585,7 @@
       <c r="B23" s="290"/>
       <c r="C23" s="296"/>
       <c r="D23" s="275" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E23" s="298"/>
       <c r="F23" s="101"/>
@@ -52882,7 +52598,7 @@
       <c r="B24" s="290"/>
       <c r="C24" s="296"/>
       <c r="D24" s="275" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E24" s="298"/>
       <c r="F24" s="101"/>
@@ -52895,7 +52611,7 @@
       <c r="B25" s="290"/>
       <c r="C25" s="296"/>
       <c r="D25" s="275" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E25" s="298"/>
       <c r="F25" s="101"/>
@@ -52908,7 +52624,7 @@
       <c r="B26" s="291"/>
       <c r="C26" s="297"/>
       <c r="D26" s="275" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E26" s="299"/>
       <c r="F26" s="70"/>
@@ -52921,7 +52637,7 @@
       <c r="B27" s="291"/>
       <c r="C27" s="297"/>
       <c r="D27" s="275" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E27" s="299"/>
       <c r="F27" s="70"/>
@@ -52932,14 +52648,14 @@
     </row>
     <row r="28" spans="1:7" ht="27" customHeight="1">
       <c r="B28" s="121" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C28" s="25" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D28" s="219"/>
       <c r="E28" s="122" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F28" s="103"/>
       <c r="G28" s="58"/>
@@ -53644,7 +53360,7 @@
     </row>
     <row r="15" spans="1:18" ht="19" customHeight="1">
       <c r="B15" s="12" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C15" s="12"/>
       <c r="D15" s="12"/>
@@ -53660,7 +53376,7 @@
     </row>
     <row r="16" spans="1:18" s="5" customFormat="1" ht="19" customHeight="1">
       <c r="B16" s="22" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C16" s="12"/>
       <c r="D16" s="12"/>
@@ -53672,7 +53388,7 @@
       <c r="J16" s="12"/>
       <c r="K16" s="12"/>
       <c r="L16" s="489" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="M16" s="489"/>
       <c r="N16" s="489"/>
@@ -53705,7 +53421,7 @@
       <c r="U17" s="65"/>
       <c r="V17" s="65"/>
       <c r="AA17" s="489" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="AB17" s="489"/>
       <c r="AC17" s="489"/>
@@ -53725,25 +53441,25 @@
       <c r="J18" s="68"/>
       <c r="K18" s="107"/>
       <c r="L18" s="83" t="s">
+        <v>223</v>
+      </c>
+      <c r="M18" s="83" t="s">
+        <v>224</v>
+      </c>
+      <c r="N18" s="83" t="s">
         <v>225</v>
       </c>
-      <c r="M18" s="83" t="s">
+      <c r="O18" s="83" t="s">
         <v>226</v>
       </c>
-      <c r="N18" s="83" t="s">
+      <c r="P18" s="83" t="s">
         <v>227</v>
       </c>
-      <c r="O18" s="83" t="s">
+      <c r="Q18" s="83" t="s">
         <v>228</v>
       </c>
-      <c r="P18" s="83" t="s">
+      <c r="R18" s="83" t="s">
         <v>229</v>
-      </c>
-      <c r="Q18" s="83" t="s">
-        <v>230</v>
-      </c>
-      <c r="R18" s="83" t="s">
-        <v>231</v>
       </c>
       <c r="S18" s="65"/>
       <c r="T18" s="65"/>
@@ -53760,12 +53476,12 @@
       <c r="B19" s="106"/>
       <c r="C19" s="106"/>
       <c r="D19" s="486" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E19" s="487"/>
       <c r="F19" s="488"/>
       <c r="G19" s="486" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="H19" s="487"/>
       <c r="I19" s="488"/>
@@ -53780,29 +53496,29 @@
       <c r="R19" s="83"/>
       <c r="S19" s="65"/>
       <c r="T19" s="486" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="U19" s="487"/>
       <c r="V19" s="488"/>
       <c r="W19" s="486" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="X19" s="487"/>
       <c r="Y19" s="488"/>
       <c r="AA19" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="AB19" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="AC19" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="AD19" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="AB19" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="AC19" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="AD19" s="1" t="s">
-        <v>238</v>
-      </c>
       <c r="AE19" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" spans="1:31" ht="15" customHeight="1">
@@ -53810,22 +53526,22 @@
       <c r="B20" s="106"/>
       <c r="C20" s="106"/>
       <c r="D20" s="167" t="s">
+        <v>237</v>
+      </c>
+      <c r="E20" s="168" t="s">
+        <v>238</v>
+      </c>
+      <c r="F20" s="169" t="s">
         <v>239</v>
       </c>
-      <c r="E20" s="168" t="s">
-        <v>240</v>
-      </c>
-      <c r="F20" s="169" t="s">
-        <v>241</v>
-      </c>
       <c r="G20" s="167" t="s">
+        <v>237</v>
+      </c>
+      <c r="H20" s="168" t="s">
+        <v>238</v>
+      </c>
+      <c r="I20" s="169" t="s">
         <v>239</v>
-      </c>
-      <c r="H20" s="168" t="s">
-        <v>240</v>
-      </c>
-      <c r="I20" s="169" t="s">
-        <v>241</v>
       </c>
       <c r="J20" s="62"/>
       <c r="K20" s="108"/>
@@ -53838,19 +53554,19 @@
       <c r="R20" s="83"/>
       <c r="S20" s="65"/>
       <c r="T20" s="256" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="U20" s="257" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="V20" s="258" t="s">
         <v>35</v>
       </c>
       <c r="W20" s="256" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="X20" s="257" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="Y20" s="258" t="s">
         <v>35</v>
@@ -53866,7 +53582,7 @@
         <v>48</v>
       </c>
       <c r="B21" s="110" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C21" s="163"/>
       <c r="D21" s="174">
@@ -53906,7 +53622,7 @@
     <row r="22" spans="1:31" ht="28" customHeight="1">
       <c r="A22" s="65"/>
       <c r="B22" s="112" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C22" s="164"/>
       <c r="D22" s="174">
@@ -53946,7 +53662,7 @@
     <row r="23" spans="1:31" ht="28" customHeight="1">
       <c r="A23" s="65"/>
       <c r="B23" s="112" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C23" s="164"/>
       <c r="D23" s="174">
@@ -54114,7 +53830,7 @@
     <row r="26" spans="1:31" s="5" customFormat="1" ht="17" customHeight="1">
       <c r="A26" s="65"/>
       <c r="B26" s="230" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C26" s="231"/>
       <c r="D26" s="232"/>

</xml_diff>